<commit_message>
Remove nature folder, fix figure 2 labels, fix figure 4 order
</commit_message>
<xml_diff>
--- a/other-data/Manuscript Figure Correspondence.xlsx
+++ b/other-data/Manuscript Figure Correspondence.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielpazsm/Library/CloudStorage/GoogleDrive-ga.paz.mota@gmail.com/My Drive/Projects/Análises/bri-analysis-pp/other-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E825C69-5100-BF4F-B905-FB64AF051FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725AEC7B-12CB-694F-9475-B6A5E06B03F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="18460" activeTab="1" xr2:uid="{11E87C29-AD34-DD44-ADB5-10354E0E7B5E}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="16660" xr2:uid="{11E87C29-AD34-DD44-ADB5-10354E0E7B5E}"/>
   </bookViews>
   <sheets>
     <sheet name="preprint" sheetId="1" r:id="rId1"/>
-    <sheet name="nature" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="66">
   <si>
     <t>/specification-curve-without-method.png</t>
   </si>
@@ -219,136 +218,22 @@
     <t>/_manuscript figures and tables/tables/Table S20.docx</t>
   </si>
   <si>
-    <t>Figure_1</t>
-  </si>
-  <si>
-    <t>Figure_2</t>
-  </si>
-  <si>
-    <t>Extended_Data_Figure_2</t>
-  </si>
-  <si>
-    <t>Figure_3</t>
-  </si>
-  <si>
-    <t>Extended_Data_Figure_3</t>
-  </si>
-  <si>
-    <t>Extended_Data_Figure_1</t>
-  </si>
-  <si>
-    <t>Figure_S2</t>
-  </si>
-  <si>
-    <t>Figure_S3</t>
-  </si>
-  <si>
-    <t>Figure_S1</t>
-  </si>
-  <si>
-    <t>Figure_S4</t>
-  </si>
-  <si>
-    <t>Figure_S5</t>
-  </si>
-  <si>
-    <t>Figure_S6</t>
-  </si>
-  <si>
-    <t>Figure_S7</t>
-  </si>
-  <si>
-    <t>Extended_Data_Figure_4</t>
-  </si>
-  <si>
-    <t>Extended_Data_Table_2</t>
-  </si>
-  <si>
-    <t>Extended_Data_Table_1</t>
-  </si>
-  <si>
-    <t>Table_1</t>
-  </si>
-  <si>
-    <t>Table_2</t>
-  </si>
-  <si>
-    <t>Table_3</t>
-  </si>
-  <si>
-    <t>Table_S1</t>
-  </si>
-  <si>
-    <t>Table_S2</t>
-  </si>
-  <si>
-    <t>Table_S3</t>
-  </si>
-  <si>
-    <t>Table_S5</t>
-  </si>
-  <si>
-    <t>Table_S4</t>
-  </si>
-  <si>
-    <t>Table_S6</t>
-  </si>
-  <si>
-    <t>Table_S7</t>
-  </si>
-  <si>
-    <t>Table_S8</t>
-  </si>
-  <si>
-    <t>Table_S9</t>
-  </si>
-  <si>
-    <t>Table_S10</t>
-  </si>
-  <si>
-    <t>Table_S11</t>
-  </si>
-  <si>
-    <t>Table_S12</t>
-  </si>
-  <si>
-    <t>Table_S13</t>
-  </si>
-  <si>
-    <t>Table_S14</t>
-  </si>
-  <si>
-    <t>Table_S15</t>
-  </si>
-  <si>
-    <t>Table_S16</t>
-  </si>
-  <si>
-    <t>Table_S17</t>
-  </si>
-  <si>
-    <t>Table_S18</t>
-  </si>
-  <si>
-    <t>Table_S19</t>
-  </si>
-  <si>
-    <t>Table_S20</t>
-  </si>
-  <si>
     <t>/_manuscript figures and tables/tables/Table S21.docx</t>
   </si>
   <si>
-    <t>Table_S21</t>
-  </si>
-  <si>
     <t>/_manuscript figures and tables/tables/Table S22.docx</t>
   </si>
   <si>
     <t>/_manuscript figures and tables/tables/Table S23.docx</t>
   </si>
   <si>
-    <t>Table_S22</t>
+    <t>S21</t>
+  </si>
+  <si>
+    <t>S22</t>
+  </si>
+  <si>
+    <t>S23</t>
   </si>
 </sst>
 </file>
@@ -404,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -415,7 +300,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75A7315-3753-2549-B467-7D63D67CE18F}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C12" sqref="A1:D39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1208,506 +1092,15 @@
       </c>
       <c r="D39" s="2"/>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E593CB48-13E5-4F72-BAFB-030523597E47}">
-  <dimension ref="A1:D42"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5" customWidth="1"/>
-    <col min="3" max="3" width="68.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D39" s="2"/>
-    </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1715,10 +1108,10 @@
         <v>24</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1726,10 +1119,10 @@
         <v>24</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove nature from figure correspondence
</commit_message>
<xml_diff>
--- a/other-data/Manuscript Figure Correspondence.xlsx
+++ b/other-data/Manuscript Figure Correspondence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielpazsm/Library/CloudStorage/GoogleDrive-ga.paz.mota@gmail.com/My Drive/Projects/Análises/bri-analysis-pp/other-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725AEC7B-12CB-694F-9475-B6A5E06B03F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C713B6-5CAF-E84A-A65B-158204F5E3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="16660" xr2:uid="{11E87C29-AD34-DD44-ADB5-10354E0E7B5E}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="18460" xr2:uid="{11E87C29-AD34-DD44-ADB5-10354E0E7B5E}"/>
   </bookViews>
   <sheets>
     <sheet name="preprint" sheetId="1" r:id="rId1"/>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75A7315-3753-2549-B467-7D63D67CE18F}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add table s24 to correspondence
</commit_message>
<xml_diff>
--- a/other-data/Manuscript Figure Correspondence.xlsx
+++ b/other-data/Manuscript Figure Correspondence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielpazsm/Library/CloudStorage/GoogleDrive-ga.paz.mota@gmail.com/My Drive/Projects/Análises/bri-analysis-pp/other-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A96817E-9AF5-834F-B4BC-5583B457CF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8A8F95-947A-6044-83DC-2ECFD99B37E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="16660" xr2:uid="{11E87C29-AD34-DD44-ADB5-10354E0E7B5E}"/>
   </bookViews>
@@ -642,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75A7315-3753-2549-B467-7D63D67CE18F}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update manuscript correspondence and fix Fig S8 pyramid
</commit_message>
<xml_diff>
--- a/other-data/Manuscript Figure Correspondence.xlsx
+++ b/other-data/Manuscript Figure Correspondence.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielpazsm/Library/CloudStorage/GoogleDrive-ga.paz.mota@gmail.com/My Drive/Projects/Análises/bri-analysis-pp/other-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8A8F95-947A-6044-83DC-2ECFD99B37E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACC803D-C893-6A42-93F2-8990FC6B00A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="16660" xr2:uid="{11E87C29-AD34-DD44-ADB5-10354E0E7B5E}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>S7</t>
   </si>
   <si>
-    <t>/all_exps_lab_units t/predictors/both/predictor x predictor - spearman.png</t>
-  </si>
-  <si>
     <t>S8</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t>/_manuscript figures and tables/tables/Table S24.docx</t>
+  </si>
+  <si>
+    <t>/all_exps_lab_units t/predictors/both/predictor x predictor (all experiments) - spearman.png</t>
   </si>
 </sst>
 </file>
@@ -643,7 +643,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -656,33 +656,33 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -693,18 +693,18 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -715,54 +715,54 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
@@ -773,373 +773,373 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1">
         <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1">
         <v>4</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>